<commit_message>
fix if the csv file has no data
</commit_message>
<xml_diff>
--- a/macro_export_summary.xlsx
+++ b/macro_export_summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>CSV NAME</t>
   </si>
@@ -28,16 +28,22 @@
     <t>Adc.c.macros.csv</t>
   </si>
   <si>
-    <t>46966</t>
+    <t>46967</t>
   </si>
   <si>
     <t>57</t>
   </si>
   <si>
+    <t>Adc.c.macros_2.csv</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>Adc_Data.c.macros.csv</t>
   </si>
   <si>
-    <t>2310</t>
+    <t>2311</t>
   </si>
   <si>
     <t>19</t>
@@ -375,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,7 +420,18 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>